<commit_message>
feat: lot 관리 - 코팅 API
</commit_message>
<xml_diff>
--- a/src/common/templates/03.Coating.xlsx
+++ b/src/common/templates/03.Coating.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\src\common\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2B6A4D-AEF5-40BC-8890-C992EEEB95DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398417DB-2071-4400-ACA5-B13D0FD83CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="645" windowWidth="17340" windowHeight="13650" xr2:uid="{1FFCD294-0548-4598-B62F-70ED7559ADF2}"/>
+    <workbookView xWindow="1815" yWindow="510" windowWidth="18060" windowHeight="14940" xr2:uid="{1FFCD294-0548-4598-B62F-70ED7559ADF2}"/>
   </bookViews>
   <sheets>
     <sheet name="코팅 작업 일지" sheetId="1" r:id="rId1"/>
@@ -30,14 +30,10 @@
     <definedName name="coatingSide3">'코팅 작업 일지'!$A$24</definedName>
     <definedName name="coatingSide4">'코팅 작업 일지'!$A$28</definedName>
     <definedName name="coatingSpeed">'코팅 작업 일지'!$G$36</definedName>
-    <definedName name="coatingSpeedFront1">'코팅 작업 일지'!$E$17</definedName>
-    <definedName name="coatingSpeedFront2">'코팅 작업 일지'!$E$21</definedName>
-    <definedName name="coatingSpeedFront3">'코팅 작업 일지'!$E$25</definedName>
-    <definedName name="coatingSpeedFront4">'코팅 작업 일지'!$E$29</definedName>
-    <definedName name="coatingSpeedRear1">'코팅 작업 일지'!$E$18</definedName>
-    <definedName name="coatingSpeedRear2">'코팅 작업 일지'!$E$22</definedName>
-    <definedName name="coatingSpeedRear3">'코팅 작업 일지'!$E$26</definedName>
-    <definedName name="coatingSpeedRear4">'코팅 작업 일지'!$E$30</definedName>
+    <definedName name="coatingWidth1">'코팅 작업 일지'!$E$16</definedName>
+    <definedName name="coatingWidth2">'코팅 작업 일지'!$E$20</definedName>
+    <definedName name="coatingWidth3">'코팅 작업 일지'!$E$24</definedName>
+    <definedName name="coatingWidth4">'코팅 작업 일지'!$E$28</definedName>
     <definedName name="equipmentCheckResult">'코팅 작업 일지'!$C$40</definedName>
     <definedName name="equipmentIssue">'코팅 작업 일지'!$K$40</definedName>
     <definedName name="inputAmount">'코팅 작업 일지'!$I$11</definedName>
@@ -52,6 +48,10 @@
     <definedName name="materialType">'코팅 작업 일지'!$A$11</definedName>
     <definedName name="materialType2">'코팅 작업 일지'!$A$13</definedName>
     <definedName name="meshFilter">'코팅 작업 일지'!$K$36</definedName>
+    <definedName name="misalignment1">'코팅 작업 일지'!$E$18</definedName>
+    <definedName name="misalignment2">'코팅 작업 일지'!$E$22</definedName>
+    <definedName name="misalignment3">'코팅 작업 일지'!$E$26</definedName>
+    <definedName name="misalignment4">'코팅 작업 일지'!$E$30</definedName>
     <definedName name="monoPumpFront1">'코팅 작업 일지'!$C$17</definedName>
     <definedName name="monoPumpFront2">'코팅 작업 일지'!$C$21</definedName>
     <definedName name="monoPumpFront3">'코팅 작업 일지'!$C$25</definedName>
@@ -164,7 +164,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
   <si>
     <t>코팅 작업 일지</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -411,6 +411,14 @@
   </si>
   <si>
     <t>7. 비고 / 특이사항</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>코팅 폭</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Miss Match</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -519,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -843,6 +851,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -853,7 +902,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -917,9 +966,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -927,9 +973,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1">
@@ -953,9 +996,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -973,15 +1013,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1060,6 +1091,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1402,8 +1466,8 @@
   </sheetPr>
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:L41"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1646,62 +1710,62 @@
       <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="28"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="73"/>
+      <c r="G15" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="35"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="36"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="19"/>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="37" t="s">
+      <c r="D16" s="35"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="38"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="19"/>
-      <c r="J16" s="37" t="s">
+      <c r="J16" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="38"/>
-      <c r="L16" s="39"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="36"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
@@ -1709,9 +1773,11 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="67"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1720,14 +1786,14 @@
       <c r="L17" s="3"/>
     </row>
     <row r="18" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="25"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -1736,46 +1802,46 @@
       <c r="L18" s="5"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="34" t="s">
+      <c r="B19" s="28"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="73"/>
+      <c r="G19" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="35"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="36"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="33"/>
     </row>
     <row r="20" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="19"/>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="19"/>
-      <c r="E20" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="37" t="s">
+      <c r="D20" s="35"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="38"/>
+      <c r="H20" s="35"/>
       <c r="I20" s="19"/>
-      <c r="J20" s="37" t="s">
+      <c r="J20" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K20" s="38"/>
-      <c r="L20" s="39"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="36"/>
     </row>
     <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
@@ -1783,9 +1849,11 @@
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="67"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1794,14 +1862,14 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="25"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -1810,46 +1878,46 @@
       <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="73"/>
+      <c r="G23" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="36"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="33"/>
     </row>
     <row r="24" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="19"/>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="19"/>
-      <c r="E24" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="37" t="s">
+      <c r="D24" s="35"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="38"/>
+      <c r="H24" s="35"/>
       <c r="I24" s="19"/>
-      <c r="J24" s="37" t="s">
+      <c r="J24" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K24" s="38"/>
-      <c r="L24" s="39"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
     </row>
     <row r="25" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
@@ -1857,9 +1925,11 @@
       </c>
       <c r="B25" s="19"/>
       <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="67"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1868,62 +1938,62 @@
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="69"/>
     </row>
     <row r="27" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="34" t="s">
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="73"/>
+      <c r="G27" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H27" s="35"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="36"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="33"/>
     </row>
     <row r="28" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="19"/>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="37" t="s">
+      <c r="D28" s="35"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="38"/>
+      <c r="H28" s="35"/>
       <c r="I28" s="19"/>
-      <c r="J28" s="37" t="s">
+      <c r="J28" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="K28" s="38"/>
-      <c r="L28" s="39"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="36"/>
     </row>
     <row r="29" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
@@ -1931,9 +2001,11 @@
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="67"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1942,14 +2014,14 @@
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="1:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
@@ -1958,157 +2030,157 @@
       <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="42"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="71"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="44"/>
-      <c r="C32" s="45" t="s">
+      <c r="B32" s="38"/>
+      <c r="C32" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="45" t="s">
+      <c r="D32" s="40"/>
+      <c r="E32" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="46"/>
-      <c r="G32" s="45" t="s">
+      <c r="F32" s="40"/>
+      <c r="G32" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="46"/>
-      <c r="I32" s="45" t="s">
+      <c r="H32" s="40"/>
+      <c r="I32" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="J32" s="46"/>
-      <c r="K32" s="45" t="s">
+      <c r="J32" s="40"/>
+      <c r="K32" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="L32" s="46"/>
+      <c r="L32" s="40"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="53" t="s">
+      <c r="B33" s="44"/>
+      <c r="C33" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="D33" s="54"/>
+      <c r="D33" s="48"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="53"/>
-      <c r="L33" s="54"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="48"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="53" t="s">
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="54"/>
+      <c r="D34" s="48"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="53"/>
-      <c r="L34" s="54"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="48"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="48"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="51"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="49" t="s">
+      <c r="A35" s="45"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="49"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="50"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="44"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="48"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="47" t="s">
+      <c r="B36" s="42"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="48"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="47" t="s">
+      <c r="F36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="J36" s="48"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="50"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="44"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="56" t="s">
+      <c r="B37" s="42"/>
+      <c r="C37" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56" t="s">
+      <c r="D37" s="50"/>
+      <c r="E37" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56" t="s">
+      <c r="F37" s="50"/>
+      <c r="G37" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="H37" s="56"/>
-      <c r="I37" s="56" t="s">
+      <c r="H37" s="50"/>
+      <c r="I37" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="J37" s="56" t="s">
+      <c r="J37" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="56"/>
+      <c r="K37" s="50"/>
       <c r="L37" s="6"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="58"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56" t="s">
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="K38" s="56"/>
+      <c r="K38" s="50"/>
       <c r="L38" s="6"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -2132,20 +2204,20 @@
         <v>54</v>
       </c>
       <c r="B40" s="14"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="56"/>
+      <c r="C40" s="51"/>
+      <c r="D40" s="50"/>
       <c r="E40" s="14" t="s">
         <v>55</v>
       </c>
       <c r="F40" s="14"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="56"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
       <c r="I40" s="14" t="s">
         <v>56</v>
       </c>
       <c r="J40" s="14"/>
-      <c r="K40" s="57"/>
-      <c r="L40" s="56"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="50"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
@@ -2168,20 +2240,20 @@
         <v>58</v>
       </c>
       <c r="B42" s="14"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
       <c r="E42" s="14" t="s">
         <v>59</v>
       </c>
       <c r="F42" s="14"/>
-      <c r="G42" s="56"/>
-      <c r="H42" s="56"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="14" t="s">
         <v>60</v>
       </c>
       <c r="J42" s="14"/>
-      <c r="K42" s="56"/>
-      <c r="L42" s="56"/>
+      <c r="K42" s="50"/>
+      <c r="L42" s="50"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
@@ -2200,105 +2272,105 @@
       <c r="L43" s="13"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="60"/>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="61"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="62"/>
+      <c r="A44" s="54"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="55"/>
+      <c r="D44" s="55"/>
+      <c r="E44" s="55"/>
+      <c r="F44" s="55"/>
+      <c r="G44" s="55"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="55"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="56"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="63"/>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="64"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="65"/>
+      <c r="A45" s="57"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="58"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58"/>
+      <c r="K45" s="58"/>
+      <c r="L45" s="59"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="63"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="64"/>
-      <c r="E46" s="64"/>
-      <c r="F46" s="64"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="64"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="65"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="58"/>
+      <c r="D46" s="58"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="58"/>
+      <c r="J46" s="58"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="59"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="63"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="64"/>
-      <c r="D47" s="64"/>
-      <c r="E47" s="64"/>
-      <c r="F47" s="64"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="64"/>
-      <c r="J47" s="64"/>
-      <c r="K47" s="64"/>
-      <c r="L47" s="65"/>
+      <c r="A47" s="57"/>
+      <c r="B47" s="58"/>
+      <c r="C47" s="58"/>
+      <c r="D47" s="58"/>
+      <c r="E47" s="58"/>
+      <c r="F47" s="58"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="58"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="58"/>
+      <c r="L47" s="59"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="63"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="64"/>
-      <c r="D48" s="64"/>
-      <c r="E48" s="64"/>
-      <c r="F48" s="64"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="64"/>
-      <c r="J48" s="64"/>
-      <c r="K48" s="64"/>
-      <c r="L48" s="65"/>
+      <c r="A48" s="57"/>
+      <c r="B48" s="58"/>
+      <c r="C48" s="58"/>
+      <c r="D48" s="58"/>
+      <c r="E48" s="58"/>
+      <c r="F48" s="58"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="58"/>
+      <c r="I48" s="58"/>
+      <c r="J48" s="58"/>
+      <c r="K48" s="58"/>
+      <c r="L48" s="59"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="63"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="64"/>
-      <c r="D49" s="64"/>
-      <c r="E49" s="64"/>
-      <c r="F49" s="64"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="64"/>
-      <c r="L49" s="65"/>
+      <c r="A49" s="57"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="58"/>
+      <c r="D49" s="58"/>
+      <c r="E49" s="58"/>
+      <c r="F49" s="58"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="58"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="58"/>
+      <c r="K49" s="58"/>
+      <c r="L49" s="59"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="66"/>
-      <c r="B50" s="67"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="67"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="67"/>
-      <c r="H50" s="67"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="67"/>
-      <c r="K50" s="67"/>
-      <c r="L50" s="68"/>
+      <c r="A50" s="60"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="62"/>
     </row>
   </sheetData>
-  <mergeCells count="152">
+  <mergeCells count="156">
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="A44:L50"/>
     <mergeCell ref="K40:L40"/>
@@ -2355,7 +2427,6 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:F27"/>
     <mergeCell ref="G27:I27"/>
     <mergeCell ref="J27:L27"/>
     <mergeCell ref="A28:B28"/>
@@ -2363,6 +2434,8 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="G28:I28"/>
     <mergeCell ref="J28:L28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="E25:F25"/>
@@ -2370,8 +2443,9 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:F23"/>
     <mergeCell ref="G23:I23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:D24"/>
@@ -2385,7 +2459,6 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="J19:L19"/>
     <mergeCell ref="A20:B20"/>
@@ -2393,6 +2466,8 @@
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="J20:L20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="E17:F17"/>
@@ -2401,7 +2476,6 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="A16:B16"/>
@@ -2409,6 +2483,8 @@
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="J16:L16"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>

</xml_diff>